<commit_message>
tentando rodar os testes
</commit_message>
<xml_diff>
--- a/php/assets/scrappedData.xlsx
+++ b/php/assets/scrappedData.xlsx
@@ -79,192 +79,192 @@
       </c>
       <c r="D1" s="0" t="inlineStr">
         <is>
-          <t>Autor 1</t>
+          <t>Author 1</t>
         </is>
       </c>
       <c r="E1" s="0" t="inlineStr">
         <is>
-          <t>Autor 1 Institution</t>
+          <t>Author 1 Institution</t>
         </is>
       </c>
       <c r="F1" s="0" t="inlineStr">
         <is>
-          <t>Autor 2</t>
+          <t>Author 2</t>
         </is>
       </c>
       <c r="G1" s="0" t="inlineStr">
         <is>
-          <t>Autor 2 Institution</t>
+          <t>Author 2 Institution</t>
         </is>
       </c>
       <c r="H1" s="0" t="inlineStr">
         <is>
-          <t>Autor 3</t>
+          <t>Author 3</t>
         </is>
       </c>
       <c r="I1" s="0" t="inlineStr">
         <is>
-          <t>Autor 3 Institution</t>
+          <t>Author 3 Institution</t>
         </is>
       </c>
       <c r="J1" s="0" t="inlineStr">
         <is>
-          <t>Autor 4</t>
+          <t>Author 4</t>
         </is>
       </c>
       <c r="K1" s="0" t="inlineStr">
         <is>
-          <t>Autor 4 Institution</t>
+          <t>Author 4 Institution</t>
         </is>
       </c>
       <c r="L1" s="0" t="inlineStr">
         <is>
-          <t>Autor 5</t>
+          <t>Author 5</t>
         </is>
       </c>
       <c r="M1" s="0" t="inlineStr">
         <is>
-          <t>Autor 5 Institution</t>
+          <t>Author 5 Institution</t>
         </is>
       </c>
       <c r="N1" s="0" t="inlineStr">
         <is>
-          <t>Autor 6</t>
+          <t>Author 6</t>
         </is>
       </c>
       <c r="O1" s="0" t="inlineStr">
         <is>
-          <t>Autor 6 Institution</t>
+          <t>Author 6 Institution</t>
         </is>
       </c>
       <c r="P1" s="0" t="inlineStr">
         <is>
-          <t>Autor 7</t>
+          <t>Author 7</t>
         </is>
       </c>
       <c r="Q1" s="0" t="inlineStr">
         <is>
-          <t>Autor 7 Institution</t>
+          <t>Author 7 Institution</t>
         </is>
       </c>
       <c r="R1" s="0" t="inlineStr">
         <is>
-          <t>Autor 8</t>
+          <t>Author 8</t>
         </is>
       </c>
       <c r="S1" s="0" t="inlineStr">
         <is>
-          <t>Autor 8 Institution</t>
+          <t>Author 8 Institution</t>
         </is>
       </c>
       <c r="T1" s="0" t="inlineStr">
         <is>
-          <t>Autor 9</t>
+          <t>Author 9</t>
         </is>
       </c>
       <c r="U1" s="0" t="inlineStr">
         <is>
-          <t>Autor 9 Institution</t>
+          <t>Author 9 Institution</t>
         </is>
       </c>
       <c r="V1" s="0" t="inlineStr">
         <is>
-          <t>Autor 10</t>
+          <t>Author 10</t>
         </is>
       </c>
       <c r="W1" s="0" t="inlineStr">
         <is>
-          <t>Autor 10 Institution</t>
+          <t>Author 10 Institution</t>
         </is>
       </c>
       <c r="X1" s="0" t="inlineStr">
         <is>
-          <t>Autor 11</t>
+          <t>Author 11</t>
         </is>
       </c>
       <c r="Y1" s="0" t="inlineStr">
         <is>
-          <t>Autor 11 Institution</t>
+          <t>Author 11 Institution</t>
         </is>
       </c>
       <c r="Z1" s="0" t="inlineStr">
         <is>
-          <t>Autor 12</t>
+          <t>Author 12</t>
         </is>
       </c>
       <c r="AA1" s="0" t="inlineStr">
         <is>
-          <t>Autor 12 Institution</t>
+          <t>Author 12 Institution</t>
         </is>
       </c>
       <c r="AB1" s="0" t="inlineStr">
         <is>
-          <t>Autor 13</t>
+          <t>Author 13</t>
         </is>
       </c>
       <c r="AC1" s="0" t="inlineStr">
         <is>
-          <t>Autor 13 Institution</t>
+          <t>Author 13 Institution</t>
         </is>
       </c>
       <c r="AD1" s="0" t="inlineStr">
         <is>
-          <t>Autor 14</t>
+          <t>Author 14</t>
         </is>
       </c>
       <c r="AE1" s="0" t="inlineStr">
         <is>
-          <t>Autor 14 Institution</t>
+          <t>Author 14 Institution</t>
         </is>
       </c>
       <c r="AF1" s="0" t="inlineStr">
         <is>
-          <t>Autor 15</t>
+          <t>Author 15</t>
         </is>
       </c>
       <c r="AG1" s="0" t="inlineStr">
         <is>
-          <t>Autor 15 Institution</t>
+          <t>Author 15 Institution</t>
         </is>
       </c>
       <c r="AH1" s="0" t="inlineStr">
         <is>
-          <t>Autor 16</t>
+          <t>Author 16</t>
         </is>
       </c>
       <c r="AI1" s="0" t="inlineStr">
         <is>
-          <t>Autor 16 Institution</t>
+          <t>Author 16 Institution</t>
         </is>
       </c>
       <c r="AJ1" s="0" t="inlineStr">
         <is>
-          <t>Autor 17</t>
+          <t>Author 17</t>
         </is>
       </c>
       <c r="AK1" s="0" t="inlineStr">
         <is>
-          <t>Autor 17 Institution</t>
+          <t>Author 17 Institution</t>
         </is>
       </c>
       <c r="AL1" s="0" t="inlineStr">
         <is>
-          <t>Autor 18</t>
+          <t>Author 18</t>
         </is>
       </c>
       <c r="AM1" s="0" t="inlineStr">
         <is>
-          <t>Autor 18 Institution</t>
+          <t>Author 18 Institution</t>
         </is>
       </c>
       <c r="AN1" s="0" t="inlineStr">
         <is>
-          <t>Autor 19</t>
+          <t>Author 19</t>
         </is>
       </c>
       <c r="AO1" s="0" t="inlineStr">
         <is>
-          <t>Autor 19 Institution</t>
+          <t>Author 19 Institution</t>
         </is>
       </c>
     </row>

</xml_diff>